<commit_message>
Added every attribute in dropdown and map, also added popup to each country with info and finished about page
</commit_message>
<xml_diff>
--- a/data/hdi.xlsx
+++ b/data/hdi.xlsx
@@ -2396,13 +2396,13 @@
   <dimension ref="A1:J189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
     <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
@@ -3439,31 +3439,31 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33">
-        <v>35.126412999999999</v>
+        <v>25.354825999999999</v>
       </c>
       <c r="D33">
-        <v>33.429859</v>
+        <v>51.183883999999999</v>
       </c>
       <c r="E33">
         <v>0.85</v>
       </c>
       <c r="F33">
-        <v>80.2</v>
+        <v>78.2</v>
       </c>
       <c r="G33">
-        <v>14</v>
+        <v>13.8</v>
       </c>
       <c r="H33">
-        <v>11.6</v>
+        <v>9.1</v>
       </c>
       <c r="I33" s="1">
-        <v>28633</v>
+        <v>123124</v>
       </c>
       <c r="J33">
-        <v>3</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -3471,31 +3471,31 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34">
-        <v>25.354825999999999</v>
+        <v>35.126412999999999</v>
       </c>
       <c r="D34">
-        <v>51.183883999999999</v>
+        <v>33.429859</v>
       </c>
       <c r="E34">
         <v>0.85</v>
       </c>
       <c r="F34">
-        <v>78.2</v>
+        <v>80.2</v>
       </c>
       <c r="G34">
-        <v>13.8</v>
+        <v>14</v>
       </c>
       <c r="H34">
-        <v>9.1</v>
+        <v>11.6</v>
       </c>
       <c r="I34" s="1">
-        <v>123124</v>
+        <v>28633</v>
       </c>
       <c r="J34">
-        <v>-31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -3599,31 +3599,31 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38">
-        <v>55.169438</v>
+        <v>35.937496000000003</v>
       </c>
       <c r="D38">
-        <v>23.881274999999999</v>
+        <v>14.375416</v>
       </c>
       <c r="E38">
         <v>0.83899999999999997</v>
       </c>
       <c r="F38">
-        <v>73.3</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="G38">
-        <v>16.399999999999999</v>
+        <v>14.4</v>
       </c>
       <c r="H38">
-        <v>12.4</v>
+        <v>10.3</v>
       </c>
       <c r="I38" s="1">
-        <v>24500</v>
+        <v>27930</v>
       </c>
       <c r="J38">
-        <v>7</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -3631,31 +3631,31 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39">
-        <v>35.937496000000003</v>
+        <v>55.169438</v>
       </c>
       <c r="D39">
-        <v>14.375416</v>
+        <v>23.881274999999999</v>
       </c>
       <c r="E39">
         <v>0.83899999999999997</v>
       </c>
       <c r="F39">
-        <v>80.599999999999994</v>
+        <v>73.3</v>
       </c>
       <c r="G39">
-        <v>14.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="H39">
-        <v>10.3</v>
+        <v>12.4</v>
       </c>
       <c r="I39" s="1">
-        <v>27930</v>
+        <v>24500</v>
       </c>
       <c r="J39">
-        <v>-1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -4015,31 +4015,31 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C51">
-        <v>53.709806999999998</v>
+        <v>61.524009999999997</v>
       </c>
       <c r="D51">
-        <v>27.953389000000001</v>
+        <v>105.31875599999999</v>
       </c>
       <c r="E51">
         <v>0.79800000000000004</v>
       </c>
       <c r="F51">
-        <v>71.3</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="G51">
-        <v>15.7</v>
+        <v>14.7</v>
       </c>
       <c r="H51">
         <v>12</v>
       </c>
       <c r="I51" s="1">
-        <v>16676</v>
+        <v>22352</v>
       </c>
       <c r="J51">
-        <v>14</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -4047,31 +4047,31 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52">
-        <v>61.524009999999997</v>
+        <v>53.709806999999998</v>
       </c>
       <c r="D52">
-        <v>105.31875599999999</v>
+        <v>27.953389000000001</v>
       </c>
       <c r="E52">
         <v>0.79800000000000004</v>
       </c>
       <c r="F52">
-        <v>70.099999999999994</v>
+        <v>71.3</v>
       </c>
       <c r="G52">
-        <v>14.7</v>
+        <v>15.7</v>
       </c>
       <c r="H52">
         <v>12</v>
       </c>
       <c r="I52" s="1">
-        <v>22352</v>
+        <v>16676</v>
       </c>
       <c r="J52">
-        <v>-1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -4111,31 +4111,31 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C54">
-        <v>45.943161000000003</v>
+        <v>-32.522779</v>
       </c>
       <c r="D54">
-        <v>24.966760000000001</v>
+        <v>-55.765835000000003</v>
       </c>
       <c r="E54">
         <v>0.79300000000000004</v>
       </c>
       <c r="F54">
-        <v>74.7</v>
+        <v>77.2</v>
       </c>
       <c r="G54">
-        <v>14.2</v>
+        <v>15.5</v>
       </c>
       <c r="H54">
-        <v>10.8</v>
+        <v>8.5</v>
       </c>
       <c r="I54" s="1">
-        <v>18108</v>
+        <v>19283</v>
       </c>
       <c r="J54">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -4143,31 +4143,31 @@
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55">
-        <v>-32.522779</v>
+        <v>45.943161000000003</v>
       </c>
       <c r="D55">
-        <v>-55.765835000000003</v>
+        <v>24.966760000000001</v>
       </c>
       <c r="E55">
         <v>0.79300000000000004</v>
       </c>
       <c r="F55">
-        <v>77.2</v>
+        <v>74.7</v>
       </c>
       <c r="G55">
-        <v>15.5</v>
+        <v>14.2</v>
       </c>
       <c r="H55">
-        <v>8.5</v>
+        <v>10.8</v>
       </c>
       <c r="I55" s="1">
-        <v>19283</v>
+        <v>18108</v>
       </c>
       <c r="J55">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -4335,31 +4335,31 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C61">
-        <v>7.5149800000000004</v>
+        <v>8.5379810000000003</v>
       </c>
       <c r="D61">
-        <v>134.58251999999999</v>
+        <v>-80.782127000000003</v>
       </c>
       <c r="E61">
         <v>0.78</v>
       </c>
       <c r="F61">
-        <v>72.7</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="G61">
-        <v>13.7</v>
+        <v>13.3</v>
       </c>
       <c r="H61">
-        <v>12.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="I61" s="1">
-        <v>13496</v>
+        <v>18192</v>
       </c>
       <c r="J61">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -4367,31 +4367,31 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C62">
-        <v>8.5379810000000003</v>
+        <v>7.5149800000000004</v>
       </c>
       <c r="D62">
-        <v>-80.782127000000003</v>
+        <v>134.58251999999999</v>
       </c>
       <c r="E62">
         <v>0.78</v>
       </c>
       <c r="F62">
-        <v>77.599999999999994</v>
+        <v>72.7</v>
       </c>
       <c r="G62">
-        <v>13.3</v>
+        <v>13.7</v>
       </c>
       <c r="H62">
-        <v>9.3000000000000007</v>
+        <v>12.3</v>
       </c>
       <c r="I62" s="1">
-        <v>18192</v>
+        <v>13496</v>
       </c>
       <c r="J62">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -4463,31 +4463,31 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C65">
-        <v>-4.6795739999999997</v>
+        <v>10.691803</v>
       </c>
       <c r="D65">
-        <v>55.491976999999999</v>
+        <v>-61.222503000000003</v>
       </c>
       <c r="E65">
         <v>0.77200000000000002</v>
       </c>
       <c r="F65">
-        <v>73.099999999999994</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="G65">
-        <v>13.4</v>
+        <v>12.3</v>
       </c>
       <c r="H65">
-        <v>9.4</v>
+        <v>10.9</v>
       </c>
       <c r="I65" s="1">
-        <v>23300</v>
+        <v>26090</v>
       </c>
       <c r="J65">
-        <v>-19</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -4495,31 +4495,31 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C66">
-        <v>10.691803</v>
+        <v>-4.6795739999999997</v>
       </c>
       <c r="D66">
-        <v>-61.222503000000003</v>
+        <v>55.491976999999999</v>
       </c>
       <c r="E66">
         <v>0.77200000000000002</v>
       </c>
       <c r="F66">
-        <v>70.400000000000006</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="G66">
-        <v>12.3</v>
+        <v>13.4</v>
       </c>
       <c r="H66">
-        <v>10.9</v>
+        <v>9.4</v>
       </c>
       <c r="I66" s="1">
-        <v>26090</v>
+        <v>23300</v>
       </c>
       <c r="J66">
-        <v>-25</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -4559,31 +4559,31 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C68">
-        <v>21.521757000000001</v>
+        <v>33.854720999999998</v>
       </c>
       <c r="D68">
-        <v>-77.781166999999996</v>
+        <v>35.862285</v>
       </c>
       <c r="E68">
         <v>0.76900000000000002</v>
       </c>
       <c r="F68">
-        <v>79.400000000000006</v>
+        <v>79.3</v>
       </c>
       <c r="G68">
         <v>13.8</v>
       </c>
       <c r="H68">
-        <v>11.5</v>
+        <v>7.9</v>
       </c>
       <c r="I68" s="1">
-        <v>7301</v>
+        <v>16509</v>
       </c>
       <c r="J68">
-        <v>47</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -4591,31 +4591,31 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C69">
-        <v>33.854720999999998</v>
+        <v>21.521757000000001</v>
       </c>
       <c r="D69">
-        <v>35.862285</v>
+        <v>-77.781166999999996</v>
       </c>
       <c r="E69">
         <v>0.76900000000000002</v>
       </c>
       <c r="F69">
-        <v>79.3</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="G69">
         <v>13.8</v>
       </c>
       <c r="H69">
-        <v>7.9</v>
+        <v>11.5</v>
       </c>
       <c r="I69" s="1">
-        <v>16509</v>
+        <v>7301</v>
       </c>
       <c r="J69">
-        <v>-1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -4623,31 +4623,31 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C70">
-        <v>9.7489170000000005</v>
+        <v>32.427908000000002</v>
       </c>
       <c r="D70">
-        <v>-83.753428</v>
+        <v>53.688046</v>
       </c>
       <c r="E70">
         <v>0.76600000000000001</v>
       </c>
       <c r="F70">
-        <v>79.400000000000006</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="G70">
-        <v>13.9</v>
+        <v>15.1</v>
       </c>
       <c r="H70">
-        <v>8.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I70" s="1">
-        <v>13413</v>
+        <v>15440</v>
       </c>
       <c r="J70">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -4655,31 +4655,31 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71">
-        <v>32.427908000000002</v>
+        <v>9.7489170000000005</v>
       </c>
       <c r="D71">
-        <v>53.688046</v>
+        <v>-83.753428</v>
       </c>
       <c r="E71">
         <v>0.76600000000000001</v>
       </c>
       <c r="F71">
-        <v>75.400000000000006</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="G71">
-        <v>15.1</v>
+        <v>13.9</v>
       </c>
       <c r="H71">
-        <v>8.1999999999999993</v>
+        <v>8.4</v>
       </c>
       <c r="I71" s="1">
-        <v>15440</v>
+        <v>13413</v>
       </c>
       <c r="J71">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -5167,31 +5167,31 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C87">
-        <v>40.069099000000001</v>
+        <v>43.915886</v>
       </c>
       <c r="D87">
-        <v>45.038189000000003</v>
+        <v>17.679075999999998</v>
       </c>
       <c r="E87">
         <v>0.73299999999999998</v>
       </c>
       <c r="F87">
-        <v>74.7</v>
+        <v>76.5</v>
       </c>
       <c r="G87">
-        <v>12.3</v>
+        <v>13.6</v>
       </c>
       <c r="H87">
-        <v>10.9</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I87" s="1">
-        <v>8124</v>
+        <v>9638</v>
       </c>
       <c r="J87">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -5199,31 +5199,31 @@
         <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C88">
-        <v>43.915886</v>
+        <v>40.069099000000001</v>
       </c>
       <c r="D88">
-        <v>17.679075999999998</v>
+        <v>45.038189000000003</v>
       </c>
       <c r="E88">
         <v>0.73299999999999998</v>
       </c>
       <c r="F88">
-        <v>76.5</v>
+        <v>74.7</v>
       </c>
       <c r="G88">
-        <v>13.6</v>
+        <v>12.3</v>
       </c>
       <c r="H88">
-        <v>8.3000000000000007</v>
+        <v>10.9</v>
       </c>
       <c r="I88" s="1">
-        <v>9638</v>
+        <v>8124</v>
       </c>
       <c r="J88">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -5327,31 +5327,31 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C92">
-        <v>-16.578192999999999</v>
+        <v>46.862496</v>
       </c>
       <c r="D92">
-        <v>179.414413</v>
+        <v>103.846656</v>
       </c>
       <c r="E92">
         <v>0.72699999999999998</v>
       </c>
       <c r="F92">
-        <v>70</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="G92">
-        <v>15.7</v>
+        <v>14.6</v>
       </c>
       <c r="H92">
-        <v>9.9</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="I92" s="1">
-        <v>7493</v>
+        <v>10729</v>
       </c>
       <c r="J92">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -5359,31 +5359,31 @@
         <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C93">
-        <v>46.862496</v>
+        <v>-16.578192999999999</v>
       </c>
       <c r="D93">
-        <v>103.846656</v>
+        <v>179.414413</v>
       </c>
       <c r="E93">
         <v>0.72699999999999998</v>
       </c>
       <c r="F93">
-        <v>69.400000000000006</v>
+        <v>70</v>
       </c>
       <c r="G93">
-        <v>14.6</v>
+        <v>15.7</v>
       </c>
       <c r="H93">
-        <v>9.3000000000000007</v>
+        <v>9.9</v>
       </c>
       <c r="I93" s="1">
-        <v>10729</v>
+        <v>7493</v>
       </c>
       <c r="J93">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -5423,31 +5423,31 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C95">
-        <v>15.414999</v>
+        <v>26.335100000000001</v>
       </c>
       <c r="D95">
-        <v>-61.370975999999999</v>
+        <v>17.228331000000001</v>
       </c>
       <c r="E95">
         <v>0.72399999999999998</v>
       </c>
       <c r="F95">
-        <v>77.8</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="G95">
-        <v>12.7</v>
+        <v>14</v>
       </c>
       <c r="H95">
-        <v>7.9</v>
+        <v>7.3</v>
       </c>
       <c r="I95" s="1">
-        <v>9994</v>
+        <v>14911</v>
       </c>
       <c r="J95">
-        <v>4</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -5455,31 +5455,31 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C96">
-        <v>26.335100000000001</v>
+        <v>15.414999</v>
       </c>
       <c r="D96">
-        <v>17.228331000000001</v>
+        <v>-61.370975999999999</v>
       </c>
       <c r="E96">
         <v>0.72399999999999998</v>
       </c>
       <c r="F96">
-        <v>71.599999999999994</v>
+        <v>77.8</v>
       </c>
       <c r="G96">
-        <v>14</v>
+        <v>12.7</v>
       </c>
       <c r="H96">
-        <v>7.3</v>
+        <v>7.9</v>
       </c>
       <c r="I96" s="1">
-        <v>14911</v>
+        <v>9994</v>
       </c>
       <c r="J96">
-        <v>-19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
@@ -5647,31 +5647,31 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C102">
-        <v>17.189876999999999</v>
+        <v>18.735693000000001</v>
       </c>
       <c r="D102">
-        <v>-88.497649999999993</v>
+        <v>-70.162650999999997</v>
       </c>
       <c r="E102">
         <v>0.71499999999999997</v>
       </c>
       <c r="F102">
-        <v>70</v>
+        <v>73.5</v>
       </c>
       <c r="G102">
-        <v>13.6</v>
+        <v>13.1</v>
       </c>
       <c r="H102">
-        <v>10.5</v>
+        <v>7.6</v>
       </c>
       <c r="I102" s="1">
-        <v>7614</v>
+        <v>11883</v>
       </c>
       <c r="J102">
-        <v>9</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
@@ -5679,31 +5679,31 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C103">
-        <v>18.735693000000001</v>
+        <v>17.189876999999999</v>
       </c>
       <c r="D103">
-        <v>-70.162650999999997</v>
+        <v>-88.497649999999993</v>
       </c>
       <c r="E103">
         <v>0.71499999999999997</v>
       </c>
       <c r="F103">
-        <v>73.5</v>
+        <v>70</v>
       </c>
       <c r="G103">
-        <v>13.1</v>
+        <v>13.6</v>
       </c>
       <c r="H103">
-        <v>7.6</v>
+        <v>10.5</v>
       </c>
       <c r="I103" s="1">
-        <v>11883</v>
+        <v>7614</v>
       </c>
       <c r="J103">
-        <v>-12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
@@ -6127,31 +6127,31 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C117">
-        <v>13.794185000000001</v>
+        <v>-30.559481999999999</v>
       </c>
       <c r="D117">
-        <v>-88.896529999999998</v>
+        <v>22.937505999999999</v>
       </c>
       <c r="E117">
         <v>0.66600000000000004</v>
       </c>
       <c r="F117">
-        <v>73</v>
+        <v>57.4</v>
       </c>
       <c r="G117">
-        <v>12.3</v>
+        <v>13.6</v>
       </c>
       <c r="H117">
-        <v>6.5</v>
+        <v>9.9</v>
       </c>
       <c r="I117" s="1">
-        <v>7349</v>
+        <v>12122</v>
       </c>
       <c r="J117">
-        <v>-3</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
@@ -6159,31 +6159,31 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C118">
-        <v>-30.559481999999999</v>
+        <v>13.794185000000001</v>
       </c>
       <c r="D118">
-        <v>22.937505999999999</v>
+        <v>-88.896529999999998</v>
       </c>
       <c r="E118">
         <v>0.66600000000000004</v>
       </c>
       <c r="F118">
-        <v>57.4</v>
+        <v>73</v>
       </c>
       <c r="G118">
-        <v>13.6</v>
+        <v>12.3</v>
       </c>
       <c r="H118">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="I118" s="1">
-        <v>12122</v>
+        <v>7349</v>
       </c>
       <c r="J118">
-        <v>-29</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
@@ -6447,31 +6447,31 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C127">
-        <v>31.791702000000001</v>
+        <v>-22.957640000000001</v>
       </c>
       <c r="D127">
-        <v>-7.0926200000000001</v>
+        <v>18.490410000000001</v>
       </c>
       <c r="E127">
         <v>0.628</v>
       </c>
       <c r="F127">
-        <v>74</v>
+        <v>64.8</v>
       </c>
       <c r="G127">
-        <v>11.6</v>
+        <v>11.3</v>
       </c>
       <c r="H127">
-        <v>4.4000000000000004</v>
+        <v>6.2</v>
       </c>
       <c r="I127" s="1">
-        <v>6850</v>
+        <v>9418</v>
       </c>
       <c r="J127">
-        <v>-8</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
@@ -6479,31 +6479,31 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C128">
-        <v>-22.957640000000001</v>
+        <v>31.791702000000001</v>
       </c>
       <c r="D128">
-        <v>18.490410000000001</v>
+        <v>-7.0926200000000001</v>
       </c>
       <c r="E128">
         <v>0.628</v>
       </c>
       <c r="F128">
-        <v>64.8</v>
+        <v>74</v>
       </c>
       <c r="G128">
-        <v>11.3</v>
+        <v>11.6</v>
       </c>
       <c r="H128">
-        <v>6.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I128" s="1">
-        <v>9418</v>
+        <v>6850</v>
       </c>
       <c r="J128">
-        <v>-21</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.3">
@@ -6703,31 +6703,31 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C135">
-        <v>34.802075000000002</v>
+        <v>-15.376706</v>
       </c>
       <c r="D135">
-        <v>38.996814999999998</v>
+        <v>166.959158</v>
       </c>
       <c r="E135">
         <v>0.59399999999999997</v>
       </c>
       <c r="F135">
-        <v>69.599999999999994</v>
+        <v>71.900000000000006</v>
       </c>
       <c r="G135">
-        <v>12.3</v>
+        <v>10.6</v>
       </c>
       <c r="H135">
-        <v>6.3</v>
+        <v>6.8</v>
       </c>
       <c r="I135" s="1">
-        <v>2728</v>
+        <v>2803</v>
       </c>
       <c r="J135">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
@@ -6735,31 +6735,31 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C136">
-        <v>-15.376706</v>
+        <v>34.802075000000002</v>
       </c>
       <c r="D136">
-        <v>166.959158</v>
+        <v>38.996814999999998</v>
       </c>
       <c r="E136">
         <v>0.59399999999999997</v>
       </c>
       <c r="F136">
-        <v>71.900000000000006</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="G136">
-        <v>10.6</v>
+        <v>12.3</v>
       </c>
       <c r="H136">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="I136" s="1">
-        <v>2803</v>
+        <v>2728</v>
       </c>
       <c r="J136">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
@@ -7663,31 +7663,31 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C165">
-        <v>-1.9402779999999999</v>
+        <v>1.3733329999999999</v>
       </c>
       <c r="D165">
-        <v>29.873888000000001</v>
+        <v>32.290275000000001</v>
       </c>
       <c r="E165">
         <v>0.48299999999999998</v>
       </c>
       <c r="F165">
-        <v>64.2</v>
+        <v>58.5</v>
       </c>
       <c r="G165">
-        <v>10.3</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H165">
-        <v>3.7</v>
+        <v>5.4</v>
       </c>
       <c r="I165" s="1">
-        <v>1458</v>
+        <v>1613</v>
       </c>
       <c r="J165">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.3">
@@ -7695,31 +7695,31 @@
         <v>163</v>
       </c>
       <c r="B166" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C166">
-        <v>1.3733329999999999</v>
+        <v>-1.9402779999999999</v>
       </c>
       <c r="D166">
-        <v>32.290275000000001</v>
+        <v>29.873888000000001</v>
       </c>
       <c r="E166">
         <v>0.48299999999999998</v>
       </c>
       <c r="F166">
-        <v>58.5</v>
+        <v>64.2</v>
       </c>
       <c r="G166">
-        <v>9.8000000000000007</v>
+        <v>10.3</v>
       </c>
       <c r="H166">
-        <v>5.4</v>
+        <v>3.7</v>
       </c>
       <c r="I166" s="1">
-        <v>1613</v>
+        <v>1458</v>
       </c>
       <c r="J166">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.3">
@@ -8459,6 +8459,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:J189">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>